<commit_message>
fixed notes tab rearraned not working properly
</commit_message>
<xml_diff>
--- a/Docs/test_plan_testing.xlsx
+++ b/Docs/test_plan_testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cuauh\OneDrive\Escritorio\Minerva\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F7302B-874A-4A69-8341-7F3670A395AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E679F1-F3BD-4D4B-BEBB-8484ED6FB96F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{433BE259-C103-4F37-9CC8-4E415CB8635F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="133">
   <si>
     <t>voice notes</t>
   </si>
@@ -62,54 +62,24 @@
     <t>failed</t>
   </si>
   <si>
-    <t>bug already fixed</t>
-  </si>
-  <si>
     <t>Typed note</t>
   </si>
   <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>when you click create on new tab popup nothing happens</t>
-  </si>
-  <si>
-    <t>cant test until scenario 1 is fixed</t>
-  </si>
-  <si>
     <t>passed</t>
   </si>
   <si>
     <t>it works</t>
   </si>
   <si>
-    <t>it lets you click the add note button and adds nothing  to the audio note</t>
-  </si>
-  <si>
     <t>Edit notes</t>
   </si>
   <si>
     <t>edit image notes is not suported yet</t>
   </si>
   <si>
-    <t xml:space="preserve"> 3  Edit Moved</t>
-  </si>
-  <si>
-    <t>2 Edit</t>
-  </si>
-  <si>
-    <t>Only 1</t>
-  </si>
-  <si>
-    <t>4 Edit Graphics</t>
-  </si>
-  <si>
-    <t>5 Edit 2 graphics</t>
-  </si>
-  <si>
-    <t>6 Edit Moved Graphics note</t>
-  </si>
-  <si>
     <t>Editor</t>
   </si>
   <si>
@@ -396,13 +366,82 @@
   </si>
   <si>
     <t>if you have the editor split and then pass a note to the editor it crashes</t>
+  </si>
+  <si>
+    <t>Reorder Chat tabs and add a chat</t>
+  </si>
+  <si>
+    <t>Reorder Chat tabs</t>
+  </si>
+  <si>
+    <t>Reorder Editor tabs</t>
+  </si>
+  <si>
+    <t>Reorder editor tabs and edit a text document</t>
+  </si>
+  <si>
+    <t>Reorder editor tabs and edit a graphics document</t>
+  </si>
+  <si>
+    <t>Reorder Notes tabs and add a note</t>
+  </si>
+  <si>
+    <t>Reorder note tabs</t>
+  </si>
+  <si>
+    <t>Enter a new note in a blank tab</t>
+  </si>
+  <si>
+    <t>it creates the note</t>
+  </si>
+  <si>
+    <t>Enter a new note in a new blank tab.</t>
+  </si>
+  <si>
+    <t>created the tab and note no problem</t>
+  </si>
+  <si>
+    <t>Enter a new note in a tab with other notes.</t>
+  </si>
+  <si>
+    <t>nter a new note in a second tab with other notes.</t>
+  </si>
+  <si>
+    <t>Enter a new voice note.</t>
+  </si>
+  <si>
+    <t>Enter a new voice note, but click add note before the task has finished processing microphone input.</t>
+  </si>
+  <si>
+    <t>the add note button get disabled when recording audio</t>
+  </si>
+  <si>
+    <t>Only 1:  A new project with a single text note.  Edit the single text note.</t>
+  </si>
+  <si>
+    <t>Edit 2: Edit 2 text notes back to back.</t>
+  </si>
+  <si>
+    <t>Edit Moved: Move a text note between tabs and edit it.</t>
+  </si>
+  <si>
+    <t>Edit Graphics: Edit a graphics note.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Edit 2 graphics: Edit 2 graphics notes back to back.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Edit Moved Graphics note: Edit a graphics note moved between tabs.</t>
+  </si>
+  <si>
+    <t>Got a StackOverflow error on MemoryTabs.gd line 445 func _on_tab_hovered it looks like the function gets called every frame (commenting the function seems to fix the issue, not sure what the function is used for, I believe it was redundant anyway)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -414,6 +453,12 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -460,6 +505,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{48AA8C2B-3B40-4051-AAF6-114539E74C2B}" name="Tabla1" displayName="Tabla1" ref="A1:E57" totalsRowShown="0">
+  <autoFilter ref="A1:E57" xr:uid="{48AA8C2B-3B40-4051-AAF6-114539E74C2B}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{7FCBE1AA-E555-4631-B8D1-4FA321022596}" name="tabname"/>
+    <tableColumn id="2" xr3:uid="{1687DB2C-F1F8-464C-823F-FACE475A8E14}" name="test title"/>
+    <tableColumn id="3" xr3:uid="{941923F1-F6F3-460E-AD3C-4623EC9334AA}" name="scenario"/>
+    <tableColumn id="4" xr3:uid="{2EFD7026-0786-45EC-901F-1857559BBB83}" name="passed/failed"/>
+    <tableColumn id="5" xr3:uid="{40B8A9D2-80C7-49F6-9C23-821901F9F8A4}" name="notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -779,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC5B4FC8-8412-4651-8D7C-4EE797771C32}">
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -791,7 +850,7 @@
     <col min="2" max="2" width="30.21875" customWidth="1"/>
     <col min="3" max="3" width="82.21875" customWidth="1"/>
     <col min="4" max="4" width="16.88671875" customWidth="1"/>
-    <col min="5" max="5" width="64" customWidth="1"/>
+    <col min="5" max="5" width="128.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -816,30 +875,30 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
+        <v>111</v>
+      </c>
+      <c r="C2" t="s">
+        <v>110</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
+        <v>112</v>
+      </c>
+      <c r="C3" t="s">
+        <v>113</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -847,845 +906,900 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
+        <v>112</v>
+      </c>
+      <c r="C4" t="s">
+        <v>114</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
+        <v>116</v>
+      </c>
+      <c r="C5" t="s">
+        <v>115</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>117</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>119</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>121</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>122</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>123</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>124</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>126</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>127</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>128</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>129</v>
       </c>
       <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
         <v>13</v>
-      </c>
-      <c r="E15" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>130</v>
       </c>
       <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
         <v>13</v>
-      </c>
-      <c r="E16" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>131</v>
       </c>
       <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" t="s">
         <v>13</v>
-      </c>
-      <c r="E17" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" t="s">
-        <v>31</v>
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>34</v>
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D21" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="D22" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" t="s">
-        <v>42</v>
+        <v>10</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="D23" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E23" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="D24" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="D25" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E25" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="D26" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E26" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="D27" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E27" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="D28" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
+        <v>40</v>
+      </c>
+      <c r="C29" t="s">
+        <v>41</v>
       </c>
       <c r="D29" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="E29" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="C30" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="D30" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E30" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="C31" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="D31" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E31" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="B32" t="s">
-        <v>67</v>
-      </c>
-      <c r="C32" t="s">
-        <v>68</v>
+        <v>48</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="E32" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="C33" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="D33" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E33" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="B34" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="C34" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="D34" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E34" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="B35" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C35" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="D35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E35" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C36" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="D36" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E36" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B37" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="C37" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="D37" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E37" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B38" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="C38" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="D38" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E38" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="B39" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="C39" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="D39" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E39" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="B40" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="C40" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="D40" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E40" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="B41" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="C41" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="D41" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="E41" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="B42" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="C42" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="D42" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="E42" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="B43" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="C43" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="D43" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="E43" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B44" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="C44" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="D44" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B45" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="C45" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="D45" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B46" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C46" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="D46" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B47" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C47" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="D47" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B48" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C48" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="D48" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B49" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="C49" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="D49" t="s">
-        <v>103</v>
-      </c>
-      <c r="E49" t="s">
-        <v>106</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>79</v>
+      </c>
+      <c r="B50" t="s">
+        <v>86</v>
+      </c>
+      <c r="C50" t="s">
         <v>89</v>
       </c>
-      <c r="B50" t="s">
-        <v>104</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="D50" t="s">
-        <v>7</v>
-      </c>
-      <c r="E50" t="s">
-        <v>107</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="B51" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="C51" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D51" t="s">
-        <v>7</v>
-      </c>
-      <c r="E51" t="s">
-        <v>111</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="B52" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="C52" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="D52" t="s">
-        <v>13</v>
+        <v>93</v>
+      </c>
+      <c r="E52" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="B53" t="s">
-        <v>114</v>
-      </c>
-      <c r="C53" t="s">
-        <v>115</v>
+        <v>94</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="D53" t="s">
         <v>7</v>
       </c>
       <c r="E53" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B54" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="C54" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="D54" t="s">
         <v>7</v>
       </c>
       <c r="E54" t="s">
-        <v>119</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>98</v>
+      </c>
+      <c r="B55" t="s">
+        <v>103</v>
+      </c>
+      <c r="C55" t="s">
+        <v>102</v>
+      </c>
+      <c r="D55" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>98</v>
+      </c>
+      <c r="B56" t="s">
+        <v>104</v>
+      </c>
+      <c r="C56" t="s">
+        <v>105</v>
+      </c>
+      <c r="D56" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>98</v>
+      </c>
+      <c r="B57" t="s">
+        <v>107</v>
+      </c>
+      <c r="C57" t="s">
+        <v>108</v>
+      </c>
+      <c r="D57" t="s">
+        <v>7</v>
+      </c>
+      <c r="E57" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>